<commit_message>
Cambios algoritmo de Lundeby
</commit_message>
<xml_diff>
--- a/Validación del cálculo de los descriptores/Parámetros python tercios.xlsx
+++ b/Validación del cálculo de los descriptores/Parámetros python tercios.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/90727fd8e92db46b/Desktop/Tesis/blind-estimation-of-acoustics-parameters/Validación del cálculo de los descriptores/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_23F921ED769B8F92AD6ADCDDE531EB3A74527C67" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BE5B764-7498-4960-AF79-DBCFD663D102}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -103,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,19 +161,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -221,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -253,27 +239,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,24 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -498,23 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F141"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.26953125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +475,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -542,7 +483,7 @@
         <v>125</v>
       </c>
       <c r="C2">
-        <v>0.95499999999999996</v>
+        <v>0.955</v>
       </c>
       <c r="D2">
         <v>-7.1</v>
@@ -554,7 +495,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -562,19 +503,19 @@
         <v>250</v>
       </c>
       <c r="C3">
-        <v>0.98099999999999998</v>
+        <v>0.981</v>
       </c>
       <c r="D3">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="E3">
-        <v>4.1500000000000004</v>
+        <v>4.15</v>
       </c>
       <c r="F3">
         <v>49.5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -594,7 +535,7 @@
         <v>38.6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -605,16 +546,16 @@
         <v>0.97</v>
       </c>
       <c r="D5">
-        <v>1.1499999999999999</v>
+        <v>1.15</v>
       </c>
       <c r="E5">
-        <v>1.1499999999999999</v>
+        <v>1.15</v>
       </c>
       <c r="F5">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -622,7 +563,7 @@
         <v>2000</v>
       </c>
       <c r="C6">
-        <v>0.96599999999999997</v>
+        <v>0.966</v>
       </c>
       <c r="D6">
         <v>2.75</v>
@@ -634,7 +575,7 @@
         <v>52.5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -654,7 +595,7 @@
         <v>53.6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -662,19 +603,19 @@
         <v>8000</v>
       </c>
       <c r="C8">
-        <v>0.98599999999999999</v>
+        <v>0.986</v>
       </c>
       <c r="D8">
-        <v>4.1900000000000004</v>
+        <v>4.19</v>
       </c>
       <c r="E8">
-        <v>4.1900000000000004</v>
+        <v>4.19</v>
       </c>
       <c r="F8">
         <v>58.7</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -694,7 +635,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -702,19 +643,19 @@
         <v>250</v>
       </c>
       <c r="C10">
-        <v>2.1230000000000002</v>
+        <v>2.123</v>
       </c>
       <c r="D10">
-        <v>-9.5500000000000007</v>
+        <v>-9.550000000000001</v>
       </c>
       <c r="E10">
-        <v>-9.5500000000000007</v>
+        <v>-9.550000000000001</v>
       </c>
       <c r="F10">
         <v>6.1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -722,19 +663,19 @@
         <v>500</v>
       </c>
       <c r="C11">
-        <v>1.9510000000000001</v>
+        <v>1.951</v>
       </c>
       <c r="D11">
-        <v>-4.6900000000000004</v>
+        <v>-4.69</v>
       </c>
       <c r="E11">
-        <v>-4.6900000000000004</v>
+        <v>-4.69</v>
       </c>
       <c r="F11">
         <v>19.5</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -742,7 +683,7 @@
         <v>1000</v>
       </c>
       <c r="C12">
-        <v>2.0590000000000002</v>
+        <v>2.059</v>
       </c>
       <c r="D12">
         <v>-1.69</v>
@@ -754,7 +695,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -774,7 +715,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -782,7 +723,7 @@
         <v>4000</v>
       </c>
       <c r="C14">
-        <v>2.0030000000000001</v>
+        <v>2.003</v>
       </c>
       <c r="D14">
         <v>-0.53</v>
@@ -794,7 +735,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -805,16 +746,16 @@
         <v>2.02</v>
       </c>
       <c r="D15">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="E15">
-        <v>-7.0000000000000007E-2</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="F15">
-        <v>38.200000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+        <v>38.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -834,7 +775,7 @@
         <v>10.4</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -854,7 +795,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -874,7 +815,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -882,7 +823,7 @@
         <v>1000</v>
       </c>
       <c r="C19">
-        <v>1.8009999999999999</v>
+        <v>1.801</v>
       </c>
       <c r="D19">
         <v>-1.39</v>
@@ -894,7 +835,7 @@
         <v>21.2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -914,7 +855,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -922,7 +863,7 @@
         <v>4000</v>
       </c>
       <c r="C21">
-        <v>1.7769999999999999</v>
+        <v>1.777</v>
       </c>
       <c r="D21">
         <v>-1.07</v>
@@ -931,10 +872,10 @@
         <v>-1.07</v>
       </c>
       <c r="F21">
-        <v>32.700000000000003</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>32.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -942,7 +883,7 @@
         <v>8000</v>
       </c>
       <c r="C22">
-        <v>1.8080000000000001</v>
+        <v>1.808</v>
       </c>
       <c r="D22">
         <v>-0.2</v>
@@ -951,10 +892,10 @@
         <v>-0.2</v>
       </c>
       <c r="F22">
-        <v>32.200000000000003</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+        <v>32.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -962,19 +903,19 @@
         <v>125</v>
       </c>
       <c r="C23">
-        <v>0.93799999999999994</v>
+        <v>0.9379999999999999</v>
       </c>
       <c r="D23">
-        <v>-4.6500000000000004</v>
+        <v>-4.65</v>
       </c>
       <c r="E23">
-        <v>-4.6500000000000004</v>
+        <v>-4.65</v>
       </c>
       <c r="F23">
         <v>5.4</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -994,7 +935,7 @@
         <v>42.3</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1002,7 +943,7 @@
         <v>500</v>
       </c>
       <c r="C25">
-        <v>1.0900000000000001</v>
+        <v>1.09</v>
       </c>
       <c r="D25">
         <v>2.48</v>
@@ -1014,7 +955,7 @@
         <v>43.3</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +975,7 @@
         <v>48.9</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1042,7 +983,7 @@
         <v>2000</v>
       </c>
       <c r="C27">
-        <v>0.97499999999999998</v>
+        <v>0.975</v>
       </c>
       <c r="D27">
         <v>2.98</v>
@@ -1054,7 +995,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1074,7 +1015,7 @@
         <v>45.7</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1082,7 +1023,7 @@
         <v>8000</v>
       </c>
       <c r="C29">
-        <v>0.96799999999999997</v>
+        <v>0.968</v>
       </c>
       <c r="D29">
         <v>2.02</v>
@@ -1094,7 +1035,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1043,7 @@
         <v>125</v>
       </c>
       <c r="C30">
-        <v>1.4810000000000001</v>
+        <v>1.481</v>
       </c>
       <c r="D30">
         <v>-7.43</v>
@@ -1114,7 +1055,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1134,7 +1075,7 @@
         <v>29.9</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -1154,7 +1095,7 @@
         <v>37.6</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -1162,19 +1103,19 @@
         <v>1000</v>
       </c>
       <c r="C33">
-        <v>1.5349999999999999</v>
+        <v>1.535</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>-0</v>
       </c>
       <c r="F33">
         <v>25.9</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -1194,7 +1135,7 @@
         <v>36.4</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1202,7 +1143,7 @@
         <v>4000</v>
       </c>
       <c r="C35">
-        <v>1.5169999999999999</v>
+        <v>1.517</v>
       </c>
       <c r="D35">
         <v>-0.15</v>
@@ -1214,7 +1155,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1234,7 +1175,7 @@
         <v>30.2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>11</v>
       </c>
@@ -1242,7 +1183,7 @@
         <v>125</v>
       </c>
       <c r="C37">
-        <v>2.0939999999999999</v>
+        <v>2.094</v>
       </c>
       <c r="D37">
         <v>0.24</v>
@@ -1254,7 +1195,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1215,7 @@
         <v>60.4</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -1282,7 +1223,7 @@
         <v>500</v>
       </c>
       <c r="C39">
-        <v>2.1800000000000002</v>
+        <v>2.18</v>
       </c>
       <c r="D39">
         <v>2.52</v>
@@ -1294,7 +1235,7 @@
         <v>63.3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>11</v>
       </c>
@@ -1305,16 +1246,16 @@
         <v>2.266</v>
       </c>
       <c r="D40">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="E40">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F40">
         <v>62.6</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -1322,7 +1263,7 @@
         <v>2000</v>
       </c>
       <c r="C41">
-        <v>2.1520000000000001</v>
+        <v>2.152</v>
       </c>
       <c r="D41">
         <v>3.13</v>
@@ -1334,7 +1275,7 @@
         <v>66.5</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -1351,10 +1292,10 @@
         <v>4.95</v>
       </c>
       <c r="F42">
-        <v>74.599999999999994</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+        <v>74.59999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -1374,7 +1315,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6">
       <c r="A44" t="s">
         <v>12</v>
       </c>
@@ -1382,7 +1323,7 @@
         <v>125</v>
       </c>
       <c r="C44">
-        <v>2.0819999999999999</v>
+        <v>2.082</v>
       </c>
       <c r="D44">
         <v>1.91</v>
@@ -1391,10 +1332,10 @@
         <v>1.91</v>
       </c>
       <c r="F44">
-        <v>37.799999999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37.8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" t="s">
         <v>12</v>
       </c>
@@ -1402,7 +1343,7 @@
         <v>250</v>
       </c>
       <c r="C45">
-        <v>2.0270000000000001</v>
+        <v>2.027</v>
       </c>
       <c r="D45">
         <v>6.52</v>
@@ -1414,7 +1355,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6">
       <c r="A46" t="s">
         <v>12</v>
       </c>
@@ -1434,7 +1375,7 @@
         <v>82.7</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6">
       <c r="A47" t="s">
         <v>12</v>
       </c>
@@ -1442,7 +1383,7 @@
         <v>1000</v>
       </c>
       <c r="C47">
-        <v>2.1389999999999998</v>
+        <v>2.139</v>
       </c>
       <c r="D47">
         <v>6.85</v>
@@ -1454,7 +1395,7 @@
         <v>82.7</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -1462,7 +1403,7 @@
         <v>2000</v>
       </c>
       <c r="C48">
-        <v>2.0449999999999999</v>
+        <v>2.045</v>
       </c>
       <c r="D48">
         <v>7.05</v>
@@ -1471,10 +1412,10 @@
         <v>7.05</v>
       </c>
       <c r="F48">
-        <v>83.1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+        <v>83.09999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1482,19 +1423,19 @@
         <v>4000</v>
       </c>
       <c r="C49">
-        <v>1.5740000000000001</v>
+        <v>1.574</v>
       </c>
       <c r="D49">
-        <v>9.9499999999999993</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="E49">
-        <v>9.9499999999999993</v>
+        <v>9.949999999999999</v>
       </c>
       <c r="F49">
-        <v>90.4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+        <v>90.40000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1511,10 +1452,10 @@
         <v>12.58</v>
       </c>
       <c r="F50">
-        <v>94.1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+        <v>94.09999999999999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1522,7 +1463,7 @@
         <v>125</v>
       </c>
       <c r="C51">
-        <v>2.1070000000000002</v>
+        <v>2.107</v>
       </c>
       <c r="D51">
         <v>-5.77</v>
@@ -1534,7 +1475,7 @@
         <v>11.7</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6">
       <c r="A52" t="s">
         <v>13</v>
       </c>
@@ -1554,7 +1495,7 @@
         <v>60.9</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1574,7 +1515,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1582,7 +1523,7 @@
         <v>1000</v>
       </c>
       <c r="C54">
-        <v>2.3740000000000001</v>
+        <v>2.374</v>
       </c>
       <c r="D54">
         <v>0.78</v>
@@ -1594,7 +1535,7 @@
         <v>53.8</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -1602,7 +1543,7 @@
         <v>2000</v>
       </c>
       <c r="C55">
-        <v>2.1110000000000002</v>
+        <v>2.111</v>
       </c>
       <c r="D55">
         <v>3.24</v>
@@ -1614,7 +1555,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -1634,7 +1575,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -1654,7 +1595,7 @@
         <v>68.5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1662,7 +1603,7 @@
         <v>125</v>
       </c>
       <c r="C58">
-        <v>2.5430000000000001</v>
+        <v>2.543</v>
       </c>
       <c r="D58">
         <v>-5.64</v>
@@ -1674,7 +1615,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1685,16 +1626,16 @@
         <v>2.528</v>
       </c>
       <c r="D59">
-        <v>-10.130000000000001</v>
+        <v>-10.13</v>
       </c>
       <c r="E59">
-        <v>-10.130000000000001</v>
+        <v>-10.13</v>
       </c>
       <c r="F59">
         <v>1.2</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -1702,7 +1643,7 @@
         <v>500</v>
       </c>
       <c r="C60">
-        <v>2.4569999999999999</v>
+        <v>2.457</v>
       </c>
       <c r="D60">
         <v>1.25</v>
@@ -1714,7 +1655,7 @@
         <v>51.2</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -1722,7 +1663,7 @@
         <v>1000</v>
       </c>
       <c r="C61">
-        <v>2.4580000000000002</v>
+        <v>2.458</v>
       </c>
       <c r="D61">
         <v>-0.59</v>
@@ -1734,7 +1675,7 @@
         <v>42.6</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1742,7 +1683,7 @@
         <v>2000</v>
       </c>
       <c r="C62">
-        <v>2.4319999999999999</v>
+        <v>2.432</v>
       </c>
       <c r="D62">
         <v>-3.32</v>
@@ -1754,7 +1695,7 @@
         <v>28.2</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6">
       <c r="A63" t="s">
         <v>14</v>
       </c>
@@ -1762,19 +1703,19 @@
         <v>4000</v>
       </c>
       <c r="C63">
-        <v>1.9970000000000001</v>
+        <v>1.997</v>
       </c>
       <c r="D63">
-        <v>-0.57999999999999996</v>
+        <v>-0.58</v>
       </c>
       <c r="E63">
-        <v>-0.57999999999999996</v>
+        <v>-0.58</v>
       </c>
       <c r="F63">
         <v>39.4</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6">
       <c r="A64" t="s">
         <v>14</v>
       </c>
@@ -1782,19 +1723,19 @@
         <v>8000</v>
       </c>
       <c r="C64">
-        <v>1.2290000000000001</v>
+        <v>1.229</v>
       </c>
       <c r="D64">
-        <v>-1.1499999999999999</v>
+        <v>-1.15</v>
       </c>
       <c r="E64">
-        <v>-1.1499999999999999</v>
+        <v>-1.15</v>
       </c>
       <c r="F64">
         <v>24.1</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -1814,7 +1755,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -1834,7 +1775,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -1854,7 +1795,7 @@
         <v>74.3</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
         <v>15</v>
       </c>
@@ -1862,19 +1803,19 @@
         <v>1000</v>
       </c>
       <c r="C68">
-        <v>1.1220000000000001</v>
+        <v>1.122</v>
       </c>
       <c r="D68">
-        <v>4.1100000000000003</v>
+        <v>4.11</v>
       </c>
       <c r="E68">
-        <v>4.1100000000000003</v>
+        <v>4.11</v>
       </c>
       <c r="F68">
         <v>66.7</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
         <v>15</v>
       </c>
@@ -1882,19 +1823,19 @@
         <v>2000</v>
       </c>
       <c r="C69">
-        <v>0.99199999999999999</v>
+        <v>0.992</v>
       </c>
       <c r="D69">
-        <v>1.1499999999999999</v>
+        <v>1.15</v>
       </c>
       <c r="E69">
-        <v>1.1499999999999999</v>
+        <v>1.15</v>
       </c>
       <c r="F69">
         <v>50.6</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6">
       <c r="A70" t="s">
         <v>15</v>
       </c>
@@ -1902,7 +1843,7 @@
         <v>4000</v>
       </c>
       <c r="C70">
-        <v>0.78200000000000003</v>
+        <v>0.782</v>
       </c>
       <c r="D70">
         <v>1.04</v>
@@ -1914,7 +1855,7 @@
         <v>41.7</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6">
       <c r="A71" t="s">
         <v>15</v>
       </c>
@@ -1922,7 +1863,7 @@
         <v>8000</v>
       </c>
       <c r="C71">
-        <v>0.60899999999999999</v>
+        <v>0.609</v>
       </c>
       <c r="D71">
         <v>2.73</v>
@@ -1934,7 +1875,7 @@
         <v>40.6</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -1954,7 +1895,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
         <v>16</v>
       </c>
@@ -1962,7 +1903,7 @@
         <v>250</v>
       </c>
       <c r="C73">
-        <v>1.0569999999999999</v>
+        <v>1.057</v>
       </c>
       <c r="D73">
         <v>-8.26</v>
@@ -1974,7 +1915,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
         <v>16</v>
       </c>
@@ -1994,7 +1935,7 @@
         <v>71.3</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
         <v>16</v>
       </c>
@@ -2002,7 +1943,7 @@
         <v>1000</v>
       </c>
       <c r="C75">
-        <v>1.2549999999999999</v>
+        <v>1.255</v>
       </c>
       <c r="D75">
         <v>3.36</v>
@@ -2014,7 +1955,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
         <v>16</v>
       </c>
@@ -2034,7 +1975,7 @@
         <v>47.1</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -2042,7 +1983,7 @@
         <v>4000</v>
       </c>
       <c r="C77">
-        <v>0.89400000000000002</v>
+        <v>0.894</v>
       </c>
       <c r="D77">
         <v>0.3</v>
@@ -2054,7 +1995,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
         <v>16</v>
       </c>
@@ -2062,7 +2003,7 @@
         <v>8000</v>
       </c>
       <c r="C78">
-        <v>0.67300000000000004</v>
+        <v>0.673</v>
       </c>
       <c r="D78">
         <v>2.1</v>
@@ -2071,10 +2012,10 @@
         <v>2.1</v>
       </c>
       <c r="F78">
-        <v>37.700000000000003</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+        <v>37.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
         <v>17</v>
       </c>
@@ -2085,16 +2026,16 @@
         <v>1.161</v>
       </c>
       <c r="D79">
-        <v>-4.3600000000000003</v>
+        <v>-4.36</v>
       </c>
       <c r="E79">
-        <v>-4.3600000000000003</v>
+        <v>-4.36</v>
       </c>
       <c r="F79">
         <v>0.1</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
         <v>17</v>
       </c>
@@ -2102,7 +2043,7 @@
         <v>250</v>
       </c>
       <c r="C80">
-        <v>1.3169999999999999</v>
+        <v>1.317</v>
       </c>
       <c r="D80">
         <v>-9.24</v>
@@ -2111,10 +2052,10 @@
         <v>-9.24</v>
       </c>
       <c r="F80">
-        <v>2.2999999999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+        <v>2.3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -2125,16 +2066,16 @@
         <v>1.405</v>
       </c>
       <c r="D81">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="E81">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="F81">
-        <v>66.099999999999994</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+        <v>66.09999999999999</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -2142,7 +2083,7 @@
         <v>1000</v>
       </c>
       <c r="C82">
-        <v>1.4590000000000001</v>
+        <v>1.459</v>
       </c>
       <c r="D82">
         <v>2.17</v>
@@ -2154,7 +2095,7 @@
         <v>57.3</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -2174,7 +2115,7 @@
         <v>41.6</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -2182,7 +2123,7 @@
         <v>4000</v>
       </c>
       <c r="C84">
-        <v>1.1160000000000001</v>
+        <v>1.116</v>
       </c>
       <c r="D84">
         <v>-0.86</v>
@@ -2194,7 +2135,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -2202,19 +2143,19 @@
         <v>8000</v>
       </c>
       <c r="C85">
-        <v>0.79500000000000004</v>
+        <v>0.795</v>
       </c>
       <c r="D85">
-        <v>1.1399999999999999</v>
+        <v>1.14</v>
       </c>
       <c r="E85">
-        <v>1.1399999999999999</v>
+        <v>1.14</v>
       </c>
       <c r="F85">
         <v>33.5</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6">
       <c r="A86" t="s">
         <v>18</v>
       </c>
@@ -2222,7 +2163,7 @@
         <v>125</v>
       </c>
       <c r="C86">
-        <v>2.6040000000000001</v>
+        <v>2.604</v>
       </c>
       <c r="D86">
         <v>-7.38</v>
@@ -2234,7 +2175,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6">
       <c r="A87" t="s">
         <v>18</v>
       </c>
@@ -2242,7 +2183,7 @@
         <v>250</v>
       </c>
       <c r="C87">
-        <v>2.4670000000000001</v>
+        <v>2.467</v>
       </c>
       <c r="D87">
         <v>-11.86</v>
@@ -2254,7 +2195,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6">
       <c r="A88" t="s">
         <v>18</v>
       </c>
@@ -2262,7 +2203,7 @@
         <v>500</v>
       </c>
       <c r="C88">
-        <v>2.4409999999999998</v>
+        <v>2.441</v>
       </c>
       <c r="D88">
         <v>0.85</v>
@@ -2274,7 +2215,7 @@
         <v>49.2</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6">
       <c r="A89" t="s">
         <v>18</v>
       </c>
@@ -2285,16 +2226,16 @@
         <v>2.44</v>
       </c>
       <c r="D89">
-        <v>-1.1299999999999999</v>
+        <v>-1.13</v>
       </c>
       <c r="E89">
-        <v>-1.1299999999999999</v>
+        <v>-1.13</v>
       </c>
       <c r="F89">
-        <v>39.799999999999997</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+        <v>39.8</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" t="s">
         <v>18</v>
       </c>
@@ -2314,7 +2255,7 @@
         <v>27.4</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6">
       <c r="A91" t="s">
         <v>18</v>
       </c>
@@ -2331,10 +2272,10 @@
         <v>-4</v>
       </c>
       <c r="F91">
-        <v>19.899999999999999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+        <v>19.9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
       <c r="A92" t="s">
         <v>18</v>
       </c>
@@ -2354,7 +2295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6">
       <c r="A93" t="s">
         <v>19</v>
       </c>
@@ -2362,7 +2303,7 @@
         <v>125</v>
       </c>
       <c r="C93">
-        <v>2.9209999999999998</v>
+        <v>2.921</v>
       </c>
       <c r="D93">
         <v>-7.98</v>
@@ -2374,7 +2315,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6">
       <c r="A94" t="s">
         <v>19</v>
       </c>
@@ -2382,7 +2323,7 @@
         <v>250</v>
       </c>
       <c r="C94">
-        <v>2.5960000000000001</v>
+        <v>2.596</v>
       </c>
       <c r="D94">
         <v>-12.33</v>
@@ -2391,10 +2332,10 @@
         <v>-12.33</v>
       </c>
       <c r="F94">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
       <c r="A95" t="s">
         <v>19</v>
       </c>
@@ -2402,7 +2343,7 @@
         <v>500</v>
       </c>
       <c r="C95">
-        <v>2.7490000000000001</v>
+        <v>2.749</v>
       </c>
       <c r="D95">
         <v>0.24</v>
@@ -2414,7 +2355,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6">
       <c r="A96" t="s">
         <v>19</v>
       </c>
@@ -2422,7 +2363,7 @@
         <v>1000</v>
       </c>
       <c r="C96">
-        <v>2.7149999999999999</v>
+        <v>2.715</v>
       </c>
       <c r="D96">
         <v>-1.72</v>
@@ -2431,10 +2372,10 @@
         <v>-1.72</v>
       </c>
       <c r="F96">
-        <v>36.700000000000003</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+        <v>36.7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
       <c r="A97" t="s">
         <v>19</v>
       </c>
@@ -2454,7 +2395,7 @@
         <v>25.1</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6">
       <c r="A98" t="s">
         <v>19</v>
       </c>
@@ -2462,19 +2403,19 @@
         <v>4000</v>
       </c>
       <c r="C98">
-        <v>2.2370000000000001</v>
+        <v>2.237</v>
       </c>
       <c r="D98">
-        <v>-4.5599999999999996</v>
+        <v>-4.56</v>
       </c>
       <c r="E98">
-        <v>-4.5599999999999996</v>
+        <v>-4.56</v>
       </c>
       <c r="F98">
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6">
       <c r="A99" t="s">
         <v>19</v>
       </c>
@@ -2482,7 +2423,7 @@
         <v>8000</v>
       </c>
       <c r="C99">
-        <v>1.3169999999999999</v>
+        <v>1.317</v>
       </c>
       <c r="D99">
         <v>-1.56</v>
@@ -2494,7 +2435,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6">
       <c r="A100" t="s">
         <v>20</v>
       </c>
@@ -2502,7 +2443,7 @@
         <v>125</v>
       </c>
       <c r="C100">
-        <v>0.88300000000000001</v>
+        <v>0.883</v>
       </c>
       <c r="D100">
         <v>-5.41</v>
@@ -2514,7 +2455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6">
       <c r="A101" t="s">
         <v>20</v>
       </c>
@@ -2522,7 +2463,7 @@
         <v>250</v>
       </c>
       <c r="C101">
-        <v>0.81</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D101">
         <v>-11.39</v>
@@ -2534,7 +2475,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6">
       <c r="A102" t="s">
         <v>20</v>
       </c>
@@ -2554,7 +2495,7 @@
         <v>5.3</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6">
       <c r="A103" t="s">
         <v>20</v>
       </c>
@@ -2571,10 +2512,10 @@
         <v>-2.54</v>
       </c>
       <c r="F103">
-        <v>16.100000000000001</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+        <v>16.1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6">
       <c r="A104" t="s">
         <v>20</v>
       </c>
@@ -2582,7 +2523,7 @@
         <v>2000</v>
       </c>
       <c r="C104">
-        <v>0.88100000000000001</v>
+        <v>0.881</v>
       </c>
       <c r="D104">
         <v>2.16</v>
@@ -2594,7 +2535,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6">
       <c r="A105" t="s">
         <v>20</v>
       </c>
@@ -2602,7 +2543,7 @@
         <v>4000</v>
       </c>
       <c r="C105">
-        <v>0.72599999999999998</v>
+        <v>0.726</v>
       </c>
       <c r="D105">
         <v>3.16</v>
@@ -2614,7 +2555,7 @@
         <v>15.1</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6">
       <c r="A106" t="s">
         <v>20</v>
       </c>
@@ -2622,19 +2563,19 @@
         <v>8000</v>
       </c>
       <c r="C106">
-        <v>0.57199999999999995</v>
+        <v>0.572</v>
       </c>
       <c r="D106">
-        <v>4.6100000000000003</v>
+        <v>4.61</v>
       </c>
       <c r="E106">
-        <v>4.6100000000000003</v>
+        <v>4.61</v>
       </c>
       <c r="F106">
         <v>25.8</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6">
       <c r="A107" t="s">
         <v>21</v>
       </c>
@@ -2642,19 +2583,19 @@
         <v>125</v>
       </c>
       <c r="C107">
-        <v>1.9890000000000001</v>
+        <v>1.989</v>
       </c>
       <c r="D107">
-        <v>-9.4499999999999993</v>
+        <v>-9.449999999999999</v>
       </c>
       <c r="E107">
-        <v>-9.4499999999999993</v>
+        <v>-9.449999999999999</v>
       </c>
       <c r="F107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6">
       <c r="A108" t="s">
         <v>21</v>
       </c>
@@ -2674,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6">
       <c r="A109" t="s">
         <v>21</v>
       </c>
@@ -2694,7 +2635,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6">
       <c r="A110" t="s">
         <v>21</v>
       </c>
@@ -2702,7 +2643,7 @@
         <v>1000</v>
       </c>
       <c r="C110">
-        <v>1.9930000000000001</v>
+        <v>1.993</v>
       </c>
       <c r="D110">
         <v>-6.68</v>
@@ -2714,7 +2655,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6">
       <c r="A111" t="s">
         <v>21</v>
       </c>
@@ -2734,7 +2675,7 @@
         <v>16.3</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6">
       <c r="A112" t="s">
         <v>21</v>
       </c>
@@ -2745,16 +2686,16 @@
         <v>1.548</v>
       </c>
       <c r="D112">
-        <v>-0.57999999999999996</v>
+        <v>-0.58</v>
       </c>
       <c r="E112">
-        <v>-0.57999999999999996</v>
+        <v>-0.58</v>
       </c>
       <c r="F112">
-        <v>8.8000000000000007</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8.800000000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6">
       <c r="A113" t="s">
         <v>21</v>
       </c>
@@ -2762,7 +2703,7 @@
         <v>8000</v>
       </c>
       <c r="C113">
-        <v>1.0660000000000001</v>
+        <v>1.066</v>
       </c>
       <c r="D113">
         <v>1.62</v>
@@ -2774,7 +2715,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6">
       <c r="A114" t="s">
         <v>22</v>
       </c>
@@ -2782,7 +2723,7 @@
         <v>125</v>
       </c>
       <c r="C114">
-        <v>2.4260000000000002</v>
+        <v>2.426</v>
       </c>
       <c r="D114">
         <v>-10.44</v>
@@ -2794,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6">
       <c r="A115" t="s">
         <v>22</v>
       </c>
@@ -2802,19 +2743,19 @@
         <v>250</v>
       </c>
       <c r="C115">
-        <v>2.1280000000000001</v>
+        <v>2.128</v>
       </c>
       <c r="D115">
-        <v>-16.149999999999999</v>
+        <v>-16.15</v>
       </c>
       <c r="E115">
-        <v>-16.149999999999999</v>
+        <v>-16.15</v>
       </c>
       <c r="F115">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6">
       <c r="A116" t="s">
         <v>22</v>
       </c>
@@ -2822,19 +2763,19 @@
         <v>500</v>
       </c>
       <c r="C116">
-        <v>2.2400000000000002</v>
+        <v>2.24</v>
       </c>
       <c r="D116">
-        <v>-4.8600000000000003</v>
+        <v>-4.86</v>
       </c>
       <c r="E116">
-        <v>-4.8600000000000003</v>
+        <v>-4.86</v>
       </c>
       <c r="F116">
         <v>2.5</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6">
       <c r="A117" t="s">
         <v>22</v>
       </c>
@@ -2854,7 +2795,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6">
       <c r="A118" t="s">
         <v>22</v>
       </c>
@@ -2862,19 +2803,19 @@
         <v>2000</v>
       </c>
       <c r="C118">
-        <v>2.2799999999999998</v>
+        <v>2.28</v>
       </c>
       <c r="D118">
-        <v>-2.5099999999999998</v>
+        <v>-2.51</v>
       </c>
       <c r="E118">
-        <v>-2.5099999999999998</v>
+        <v>-2.51</v>
       </c>
       <c r="F118">
         <v>13.9</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6">
       <c r="A119" t="s">
         <v>22</v>
       </c>
@@ -2894,7 +2835,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6">
       <c r="A120" t="s">
         <v>22</v>
       </c>
@@ -2914,7 +2855,7 @@
         <v>15.7</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6">
       <c r="A121" t="s">
         <v>23</v>
       </c>
@@ -2934,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6">
       <c r="A122" t="s">
         <v>23</v>
       </c>
@@ -2954,7 +2895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6">
       <c r="A123" t="s">
         <v>23</v>
       </c>
@@ -2962,7 +2903,7 @@
         <v>500</v>
       </c>
       <c r="C123">
-        <v>2.5249999999999999</v>
+        <v>2.525</v>
       </c>
       <c r="D123">
         <v>-3.86</v>
@@ -2974,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6">
       <c r="A124" t="s">
         <v>23</v>
       </c>
@@ -2982,7 +2923,7 @@
         <v>1000</v>
       </c>
       <c r="C124">
-        <v>2.4780000000000002</v>
+        <v>2.478</v>
       </c>
       <c r="D124">
         <v>-1.81</v>
@@ -2994,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6">
       <c r="A125" t="s">
         <v>23</v>
       </c>
@@ -3014,7 +2955,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6">
       <c r="A126" t="s">
         <v>23</v>
       </c>
@@ -3034,7 +2975,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6">
       <c r="A127" t="s">
         <v>23</v>
       </c>
@@ -3054,7 +2995,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6">
       <c r="A128" t="s">
         <v>24</v>
       </c>
@@ -3074,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6">
       <c r="A129" t="s">
         <v>24</v>
       </c>
@@ -3094,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6">
       <c r="A130" t="s">
         <v>24</v>
       </c>
@@ -3102,7 +3043,7 @@
         <v>500</v>
       </c>
       <c r="C130">
-        <v>2.5259999999999998</v>
+        <v>2.526</v>
       </c>
       <c r="D130">
         <v>-1.5</v>
@@ -3114,7 +3055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6">
       <c r="A131" t="s">
         <v>24</v>
       </c>
@@ -3122,7 +3063,7 @@
         <v>1000</v>
       </c>
       <c r="C131">
-        <v>2.4849999999999999</v>
+        <v>2.485</v>
       </c>
       <c r="D131">
         <v>-0.44</v>
@@ -3134,7 +3075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6">
       <c r="A132" t="s">
         <v>24</v>
       </c>
@@ -3142,7 +3083,7 @@
         <v>2000</v>
       </c>
       <c r="C132">
-        <v>2.4390000000000001</v>
+        <v>2.439</v>
       </c>
       <c r="D132">
         <v>2.1</v>
@@ -3154,7 +3095,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6">
       <c r="A133" t="s">
         <v>24</v>
       </c>
@@ -3174,7 +3115,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6">
       <c r="A134" t="s">
         <v>24</v>
       </c>
@@ -3194,7 +3135,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6">
       <c r="A135" t="s">
         <v>25</v>
       </c>
@@ -3214,7 +3155,7 @@
         <v>3.4</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6">
       <c r="A136" t="s">
         <v>25</v>
       </c>
@@ -3222,7 +3163,7 @@
         <v>250</v>
       </c>
       <c r="C136">
-        <v>0.77200000000000002</v>
+        <v>0.772</v>
       </c>
       <c r="D136">
         <v>-3.7</v>
@@ -3231,10 +3172,10 @@
         <v>-3.7</v>
       </c>
       <c r="F136">
-        <v>18.399999999999999</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+        <v>18.4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
       <c r="A137" t="s">
         <v>25</v>
       </c>
@@ -3242,7 +3183,7 @@
         <v>500</v>
       </c>
       <c r="C137">
-        <v>1.0229999999999999</v>
+        <v>1.023</v>
       </c>
       <c r="D137">
         <v>-0.63</v>
@@ -3254,7 +3195,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6">
       <c r="A138" t="s">
         <v>25</v>
       </c>
@@ -3274,7 +3215,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6">
       <c r="A139" t="s">
         <v>25</v>
       </c>
@@ -3282,7 +3223,7 @@
         <v>2000</v>
       </c>
       <c r="C139">
-        <v>0.94799999999999995</v>
+        <v>0.948</v>
       </c>
       <c r="D139">
         <v>-1.42</v>
@@ -3294,7 +3235,7 @@
         <v>35.9</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6">
       <c r="A140" t="s">
         <v>25</v>
       </c>
@@ -3302,7 +3243,7 @@
         <v>4000</v>
       </c>
       <c r="C140">
-        <v>0.80100000000000005</v>
+        <v>0.801</v>
       </c>
       <c r="D140">
         <v>2.42</v>
@@ -3314,7 +3255,7 @@
         <v>55.1</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6">
       <c r="A141" t="s">
         <v>25</v>
       </c>

</xml_diff>